<commit_message>
This is the second version. The Jira flow has been introduced as per flow diagram, tool takes the input for label from user incase parent doesn't have any
</commit_message>
<xml_diff>
--- a/Jira-Automaion-Python/automation/Issue.xlsx
+++ b/Jira-Automaion-Python/automation/Issue.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amitmittal/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74A53615-70A9-7049-9A63-8EF54FAC8047}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED4220E7-CE82-C04D-BD8B-47ACE0A9EB2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{1A905619-3492-524E-B579-C539546335C0}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="rollout" sheetId="1" r:id="rId1"/>
+    <sheet name="rapidstart" sheetId="3" r:id="rId2"/>
+    <sheet name="rapidresponse" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,52 +36,102 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="24">
   <si>
     <t>Description</t>
   </si>
   <si>
-    <t>This is test 1 from excel.</t>
-  </si>
-  <si>
-    <t>This is test 2 from excel.</t>
-  </si>
-  <si>
-    <t>This is test 3 from excel.</t>
-  </si>
-  <si>
-    <t>This is test 4 from excel.</t>
-  </si>
-  <si>
-    <t>This is test 5 from excel.</t>
-  </si>
-  <si>
     <t>Summary</t>
   </si>
   <si>
-    <t>Summary Test 1</t>
-  </si>
-  <si>
-    <t>Summary Test 2</t>
-  </si>
-  <si>
-    <t>Summary Test 3</t>
-  </si>
-  <si>
-    <t>Summary Test 4</t>
-  </si>
-  <si>
-    <t>Summary Test 5</t>
+    <t>Assignee</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Guardrail Review</t>
+  </si>
+  <si>
+    <t>Review previous deployment</t>
+  </si>
+  <si>
+    <t>Ready for Production Review</t>
+  </si>
+  <si>
+    <t>Ready for AT Review</t>
+  </si>
+  <si>
+    <t>Ready to Configure Review</t>
+  </si>
+  <si>
+    <t>Project Startup Review</t>
+  </si>
+  <si>
+    <t>61e7160a38041c006854cd45</t>
+  </si>
+  <si>
+    <t>This is a test 1</t>
+  </si>
+  <si>
+    <t>This is a test 2</t>
+  </si>
+  <si>
+    <t>This is a test 3</t>
+  </si>
+  <si>
+    <t>This is a test 4</t>
+  </si>
+  <si>
+    <t>This is a test 5</t>
+  </si>
+  <si>
+    <t>This is a test 6</t>
+  </si>
+  <si>
+    <t>Sales to Deployment Transition</t>
+  </si>
+  <si>
+    <t>Ready for UAT Review</t>
+  </si>
+  <si>
+    <t>Technical Blueprint</t>
+  </si>
+  <si>
+    <t>Solution Transfer to Support</t>
+  </si>
+  <si>
+    <t>Solution Maintenance Manual</t>
+  </si>
+  <si>
+    <t>Solution Blueprint</t>
+  </si>
+  <si>
+    <t>Performance Essentials</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF00AA00"/>
+      <name val="Menlo"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -105,8 +157,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="11" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,62 +475,344 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F357C4F-6122-814C-95CF-3613E0564507}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" activeCellId="1" sqref="C2:D7 A15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B5DD833-2327-DD48-A379-F4B8785D4EBA}">
+  <dimension ref="A1:D7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{720E4D3C-DFF9-174C-AC60-C8CFDDE4E74D}">
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="27.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>8</v>
       </c>
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
-        <v>5</v>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>